<commit_message>
detecting country and entityName
</commit_message>
<xml_diff>
--- a/Samples/dataFrameOutput.xlsx
+++ b/Samples/dataFrameOutput.xlsx
@@ -14,72 +14,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
-  <si>
-    <t>Penna</t>
-  </si>
-  <si>
-    <t>Animas</t>
-  </si>
-  <si>
-    <t>Urastar</t>
-  </si>
-  <si>
-    <t>Anico El MINES LIMITED (Ohio)</t>
-  </si>
-  <si>
-    <t>Banking</t>
-  </si>
-  <si>
-    <t>Transaction</t>
-  </si>
-  <si>
-    <t>Golden</t>
-  </si>
-  <si>
-    <t>Golden Animas</t>
-  </si>
-  <si>
-    <t>(NYSE, TSX: AEM)</t>
-  </si>
-  <si>
-    <t>Inc.</t>
-  </si>
-  <si>
-    <t>services</t>
-  </si>
-  <si>
-    <t>oppurtnity</t>
-  </si>
-  <si>
-    <t>_x000C_</t>
-  </si>
-  <si>
-    <t>(Barbados)</t>
-  </si>
-  <si>
-    <t>Inc. (Ohio)</t>
-  </si>
-  <si>
-    <t>Corp.</t>
-  </si>
-  <si>
-    <t>oppurtnity Transaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>(British</t>
-  </si>
-  <si>
-    <t>Corp. services</t>
-  </si>
-  <si>
-    <t>Columbia)</t>
-  </si>
-  <si>
-    <t>(British Inc, (Ohio)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>entityName</t>
+  </si>
+  <si>
+    <t>Barbados</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>British Columbia</t>
+  </si>
+  <si>
+    <t>British Inc, (Ohio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Penna Banking Inc. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Animas Transaction services Inc. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urastar Golden oppurtnity Corp. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urastar Golden Animas oppurtnity Transaction Corp. services </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anico El MINES LIMITED </t>
   </si>
 </sst>
 </file>
@@ -437,167 +404,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="B1" s="1">
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" t="s">
         <v>9</v>
       </c>
-      <c r="M5" t="s">
-        <v>13</v>
-      </c>
-      <c r="O5" t="s">
-        <v>17</v>
-      </c>
-      <c r="P5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -605,13 +470,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -619,13 +481,73 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
different image outputs in various sheets
</commit_message>
<xml_diff>
--- a/Samples/dataFrameOutput.xlsx
+++ b/Samples/dataFrameOutput.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet_name_1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet_name_3" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>country</t>
   </si>
@@ -22,31 +22,49 @@
     <t>entityName</t>
   </si>
   <si>
-    <t>Barbados</t>
+    <t>canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
   <si>
     <t>Ohio</t>
   </si>
   <si>
-    <t>British Columbia</t>
-  </si>
-  <si>
-    <t>British Inc, (Ohio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Penna Banking Inc. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Animas Transaction services Inc. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Urastar Golden oppurtnity Corp. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Urastar Golden Animas oppurtnity Transaction Corp. services </t>
+    <t>embados</t>
+  </si>
+  <si>
+    <t>Chie</t>
+  </si>
+  <si>
+    <t>Urastar ‘oppurinity ‘Corp.  Gries columbia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3205775 Canagian robots </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kang Matartic  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Penns Banking  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Animas Transaction Ine. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2azi4s1 ‘hie ine. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urastar ‘oppurinity ‘Corp.  Gries columbia) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      2azi4s1 ‘hie ine. </t>
   </si>
   <si>
     <t xml:space="preserve">Anico El MINES LIMITED </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Anico El MINES LIMITED </t>
   </si>
 </sst>
 </file>
@@ -404,7 +422,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -422,22 +440,16 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -445,10 +457,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -456,7 +468,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -466,44 +478,26 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -511,10 +505,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -522,10 +516,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -533,10 +527,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -544,10 +538,32 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>